<commit_message>
Implemented completed activity history
</commit_message>
<xml_diff>
--- a/converter/CSV_to_SQL/CSV_to_SQL/bin/Debug/net6.0/running MTE.xlsx
+++ b/converter/CSV_to_SQL/CSV_to_SQL/bin/Debug/net6.0/running MTE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12345\OneDrive\Stalinis kompiuteris\converter\CSV_to_SQL\CSV_to_SQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12345\OneDrive\Documents\GitHub\FitMax\converter\CSV_to_SQL\CSV_to_SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C85731-C123-4CF2-8102-F5019B791F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF03765-5457-4245-B468-2AB40DC1F300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="1305" windowWidth="14340" windowHeight="13485" xr2:uid="{E02DFD1C-5FA8-45A3-8D27-8541CCA6728D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E02DFD1C-5FA8-45A3-8D27-8541CCA6728D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,27 +188,6 @@
     <t>activity name</t>
   </si>
   <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
     <t>Daily</t>
   </si>
   <si>
@@ -216,6 +195,27 @@
   </si>
   <si>
     <t>Weekends Off (light)</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>MONDAY</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,287 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE864C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE864C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE864C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE864C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE864C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -703,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894CFDA4-9046-4071-82EC-8E16B1258843}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z49" sqref="Z49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,14 +1088,14 @@
       <c r="L2" s="2">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>58</v>
+      <c r="M2" t="s">
+        <v>50</v>
       </c>
       <c r="O2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="2">
         <f>INDEX(A:A,MATCH(PROPER(TRIM(R2)),B:B,0))</f>
@@ -868,13 +1148,13 @@
         <v>2</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="O3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" ref="Q3:Q14" si="1">INDEX(A:A,MATCH(PROPER(TRIM(R3)),B:B,0))</f>
@@ -927,13 +1207,13 @@
         <v>3</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="O4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="1"/>
@@ -983,10 +1263,10 @@
         <v>37.33</v>
       </c>
       <c r="O5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" si="1"/>
@@ -1035,10 +1315,10 @@
         <v>210</v>
       </c>
       <c r="O6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q6" s="2">
         <f t="shared" si="1"/>
@@ -1087,10 +1367,10 @@
         <v>284.38</v>
       </c>
       <c r="O7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="2">
         <f t="shared" si="1"/>
@@ -1139,10 +1419,10 @@
         <v>280</v>
       </c>
       <c r="O8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="1"/>
@@ -1191,10 +1471,10 @@
         <v>354.38</v>
       </c>
       <c r="O9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="1"/>
@@ -1243,10 +1523,10 @@
         <v>315</v>
       </c>
       <c r="O10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q10" s="2">
         <f t="shared" si="1"/>
@@ -1295,10 +1575,10 @@
         <v>420</v>
       </c>
       <c r="O11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q11" s="2">
         <f t="shared" si="1"/>
@@ -1345,10 +1625,10 @@
         <v>87.5</v>
       </c>
       <c r="O12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q12" s="2">
         <f t="shared" si="1"/>
@@ -1398,10 +1678,10 @@
         <v>14</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="1"/>
@@ -1451,10 +1731,10 @@
         <v>33.6</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q14" s="2">
         <f t="shared" si="1"/>
@@ -1504,10 +1784,10 @@
         <v>14</v>
       </c>
       <c r="O15" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q15" s="2">
         <f>INDEX(A:A,MATCH(PROPER(TRIM(R15)),B:B,0))</f>
@@ -1557,10 +1837,10 @@
         <v>21</v>
       </c>
       <c r="O16" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" ref="Q16:Q27" si="6">INDEX(A:A,MATCH(PROPER(TRIM(R16)),B:B,0))</f>
@@ -1610,10 +1890,10 @@
         <v>18.899999999999999</v>
       </c>
       <c r="O17" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q17" s="2">
         <f t="shared" si="6"/>
@@ -1663,10 +1943,10 @@
         <v>21</v>
       </c>
       <c r="O18" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q18" s="2">
         <f t="shared" si="6"/>
@@ -1716,10 +1996,10 @@
         <v>21</v>
       </c>
       <c r="O19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q19" s="2">
         <f t="shared" si="6"/>
@@ -1769,10 +2049,10 @@
         <v>21</v>
       </c>
       <c r="O20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" si="6"/>
@@ -1822,10 +2102,10 @@
         <v>14</v>
       </c>
       <c r="O21" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q21" s="2">
         <f t="shared" si="6"/>
@@ -1841,10 +2121,10 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O22" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q22" s="2">
         <f t="shared" si="6"/>
@@ -1860,10 +2140,10 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q23" s="2">
         <f t="shared" si="6"/>
@@ -1879,10 +2159,10 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O24" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q24" s="2">
         <f t="shared" si="6"/>
@@ -1898,10 +2178,10 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O25" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q25" s="2">
         <f t="shared" si="6"/>
@@ -1917,10 +2197,10 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O26" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q26" s="2">
         <f t="shared" si="6"/>
@@ -1936,10 +2216,10 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O27" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q27" s="2">
         <f t="shared" si="6"/>
@@ -1955,10 +2235,10 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O28" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q28" s="2">
         <f>INDEX(A:A,MATCH(PROPER(TRIM(R28)),B:B,0))</f>
@@ -1974,10 +2254,10 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O29" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q29" s="2">
         <f t="shared" ref="Q29:Q31" si="7">INDEX(A:A,MATCH(PROPER(TRIM(R29)),B:B,0))</f>
@@ -1993,10 +2273,10 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O30" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q30" s="2">
         <f t="shared" si="7"/>
@@ -2012,10 +2292,10 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O31" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q31" s="2">
         <f t="shared" si="7"/>
@@ -2031,10 +2311,10 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O32" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q32" s="2">
         <f t="shared" ref="Q32:Q46" si="8">INDEX(A:A,MATCH(PROPER(TRIM(R32)),B:B,0))</f>
@@ -2050,10 +2330,10 @@
     </row>
     <row r="33" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O33" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q33" s="2">
         <f t="shared" si="8"/>
@@ -2069,10 +2349,10 @@
     </row>
     <row r="34" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O34" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q34" s="2">
         <f t="shared" si="8"/>
@@ -2088,10 +2368,10 @@
     </row>
     <row r="35" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O35" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q35" s="2">
         <f t="shared" si="8"/>
@@ -2107,10 +2387,10 @@
     </row>
     <row r="36" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O36" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q36" s="2">
         <f t="shared" si="8"/>
@@ -2126,10 +2406,10 @@
     </row>
     <row r="37" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O37" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q37" s="2">
         <f t="shared" si="8"/>
@@ -2145,10 +2425,10 @@
     </row>
     <row r="38" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O38" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q38" s="2">
         <f t="shared" si="8"/>
@@ -2164,10 +2444,10 @@
     </row>
     <row r="39" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O39" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q39" s="2">
         <f t="shared" si="8"/>
@@ -2183,10 +2463,10 @@
     </row>
     <row r="40" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O40" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="Q40" s="2">
         <f t="shared" si="8"/>
@@ -2202,10 +2482,10 @@
     </row>
     <row r="41" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O41" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q41" s="2">
         <f t="shared" si="8"/>
@@ -2221,10 +2501,10 @@
     </row>
     <row r="42" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O42" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q42" s="2">
         <f t="shared" si="8"/>
@@ -2240,10 +2520,10 @@
     </row>
     <row r="43" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O43" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q43" s="2">
         <f t="shared" si="8"/>
@@ -2259,10 +2539,10 @@
     </row>
     <row r="44" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O44" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Q44" s="2">
         <f t="shared" si="8"/>
@@ -2278,10 +2558,10 @@
     </row>
     <row r="45" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O45" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Q45" s="2">
         <f t="shared" si="8"/>
@@ -2297,10 +2577,10 @@
     </row>
     <row r="46" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O46" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Q46" s="2">
         <f t="shared" si="8"/>
@@ -2320,34 +2600,54 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H1:H21 G22:G1048576">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"reps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"Monday"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+      <formula>"MONDAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
-      <formula>"Tuesday"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"TUESDAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"Wednesday"</formula>
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+      <formula>"WEDNESDAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"Thursday"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+      <formula>"THURSDAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>"Friday"</formula>
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+      <formula>"FRIDAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
-      <formula>"Saturday"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"SATURDAY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
-      <formula>"Sunday"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>"SUNDAY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
-      <formula>NOT(OR(P1="Monday", P1="Tuesday", P1="Wednesday", P1="Thursday", P1="Friday", P1="Saturday", P1="Sunday", P1="day", P1=""))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2:V46">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"MONDAY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"TUESDAY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"WEDNESDAY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"THURSDAY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>"FRIDAY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+      <formula>"SATURDAY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+      <formula>"SUNDAY"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>